<commit_message>
non-hatchert Distribution estimate figures
</commit_message>
<xml_diff>
--- a/Salmonids/data/DistributionEstimates_WOMT_WY2024.xlsx
+++ b/Salmonids/data/DistributionEstimates_WOMT_WY2024.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp.sharepoint.com/sites/bor-wy2024outlook_assessments/Shared Documents/General/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/nbertrand_usbr_gov/Documents/Desktop/Bertrand/GitHub/omr_report_2024/Salmonids/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="560" documentId="13_ncr:1_{596D66D2-391F-42CF-B008-6C712CC2D79B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84AA9212-3024-4A52-AE4A-F810F9181035}"/>
+  <xr:revisionPtr revIDLastSave="561" documentId="13_ncr:1_{596D66D2-391F-42CF-B008-6C712CC2D79B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BD1A1F2-565F-4A3D-ADB6-39C44E7A2AC0}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="749" activeTab="1" xr2:uid="{0098A3D5-292E-4E0B-8343-5C5D19D7C3A2}"/>
   </bookViews>
@@ -1659,72 +1659,6 @@
                 <c:pt idx="250">
                   <c:v>45453</c:v>
                 </c:pt>
-                <c:pt idx="251">
-                  <c:v>45454</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>45455</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>45456</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>45457</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>45458</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>45459</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>45460</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>45461</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>45462</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>45463</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>45464</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>45465</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>45466</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>45467</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>45468</c:v>
-                </c:pt>
-                <c:pt idx="266">
-                  <c:v>45469</c:v>
-                </c:pt>
-                <c:pt idx="267">
-                  <c:v>45470</c:v>
-                </c:pt>
-                <c:pt idx="268">
-                  <c:v>45471</c:v>
-                </c:pt>
-                <c:pt idx="269">
-                  <c:v>45472</c:v>
-                </c:pt>
-                <c:pt idx="270">
-                  <c:v>45473</c:v>
-                </c:pt>
-                <c:pt idx="271">
-                  <c:v>45474</c:v>
-                </c:pt>
-                <c:pt idx="272">
-                  <c:v>45475</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -3282,72 +3216,6 @@
                 <c:pt idx="250">
                   <c:v>45453</c:v>
                 </c:pt>
-                <c:pt idx="251">
-                  <c:v>45454</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>45455</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>45456</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>45457</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>45458</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>45459</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>45460</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>45461</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>45462</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>45463</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>45464</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>45465</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>45466</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>45467</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>45468</c:v>
-                </c:pt>
-                <c:pt idx="266">
-                  <c:v>45469</c:v>
-                </c:pt>
-                <c:pt idx="267">
-                  <c:v>45470</c:v>
-                </c:pt>
-                <c:pt idx="268">
-                  <c:v>45471</c:v>
-                </c:pt>
-                <c:pt idx="269">
-                  <c:v>45472</c:v>
-                </c:pt>
-                <c:pt idx="270">
-                  <c:v>45473</c:v>
-                </c:pt>
-                <c:pt idx="271">
-                  <c:v>45474</c:v>
-                </c:pt>
-                <c:pt idx="272">
-                  <c:v>45475</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -4904,72 +4772,6 @@
                 </c:pt>
                 <c:pt idx="250">
                   <c:v>45453</c:v>
-                </c:pt>
-                <c:pt idx="251">
-                  <c:v>45454</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>45455</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>45456</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>45457</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>45458</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>45459</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>45460</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>45461</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>45462</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>45463</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>45464</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>45465</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>45466</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>45467</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>45468</c:v>
-                </c:pt>
-                <c:pt idx="266">
-                  <c:v>45469</c:v>
-                </c:pt>
-                <c:pt idx="267">
-                  <c:v>45470</c:v>
-                </c:pt>
-                <c:pt idx="268">
-                  <c:v>45471</c:v>
-                </c:pt>
-                <c:pt idx="269">
-                  <c:v>45472</c:v>
-                </c:pt>
-                <c:pt idx="270">
-                  <c:v>45473</c:v>
-                </c:pt>
-                <c:pt idx="271">
-                  <c:v>45474</c:v>
-                </c:pt>
-                <c:pt idx="272">
-                  <c:v>45475</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6892,51 +6694,6 @@
                 <c:pt idx="250">
                   <c:v>45453</c:v>
                 </c:pt>
-                <c:pt idx="251">
-                  <c:v>45454</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>45455</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>45456</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>45457</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>45458</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>45459</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>45460</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>45461</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>45462</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>45463</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>45464</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>45465</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>45466</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>45467</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>45468</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -8494,51 +8251,6 @@
                 <c:pt idx="250">
                   <c:v>45453</c:v>
                 </c:pt>
-                <c:pt idx="251">
-                  <c:v>45454</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>45455</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>45456</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>45457</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>45458</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>45459</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>45460</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>45461</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>45462</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>45463</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>45464</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>45465</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>45466</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>45467</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>45468</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -10095,51 +9807,6 @@
                 </c:pt>
                 <c:pt idx="250">
                   <c:v>45453</c:v>
-                </c:pt>
-                <c:pt idx="251">
-                  <c:v>45454</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>45455</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>45456</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>45457</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>45458</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>45459</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>45460</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>45461</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>45462</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>45463</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>45464</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>45465</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>45466</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>45467</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>45468</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12032,51 +11699,6 @@
                 <c:pt idx="250">
                   <c:v>45453</c:v>
                 </c:pt>
-                <c:pt idx="251">
-                  <c:v>45454</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>45455</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>45456</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>45457</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>45458</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>45459</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>45460</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>45461</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>45462</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>45463</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>45464</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>45465</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>45466</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>45467</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>45468</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -13634,51 +13256,6 @@
                 <c:pt idx="250">
                   <c:v>45453</c:v>
                 </c:pt>
-                <c:pt idx="251">
-                  <c:v>45454</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>45455</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>45456</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>45457</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>45458</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>45459</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>45460</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>45461</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>45462</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>45463</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>45464</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>45465</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>45466</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>45467</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>45468</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -15235,51 +14812,6 @@
                 </c:pt>
                 <c:pt idx="250">
                   <c:v>45453</c:v>
-                </c:pt>
-                <c:pt idx="251">
-                  <c:v>45454</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>45455</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>45456</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>45457</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>45458</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>45459</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>45460</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>45461</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>45462</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>45463</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>45464</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>45465</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>45466</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>45467</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>45468</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17223,51 +16755,6 @@
                 <c:pt idx="250">
                   <c:v>45453</c:v>
                 </c:pt>
-                <c:pt idx="251">
-                  <c:v>45454</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>45455</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>45456</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>45457</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>45458</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>45459</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>45460</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>45461</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>45462</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>45463</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>45464</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>45465</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>45466</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>45467</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>45468</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -18825,51 +18312,6 @@
                 <c:pt idx="250">
                   <c:v>45453</c:v>
                 </c:pt>
-                <c:pt idx="251">
-                  <c:v>45454</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>45455</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>45456</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>45457</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>45458</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>45459</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>45460</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>45461</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>45462</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>45463</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>45464</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>45465</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>45466</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>45467</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>45468</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -20426,51 +19868,6 @@
                 </c:pt>
                 <c:pt idx="250">
                   <c:v>45453</c:v>
-                </c:pt>
-                <c:pt idx="251">
-                  <c:v>45454</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>45455</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>45456</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>45457</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>45458</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>45459</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>45460</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>45461</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>45462</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>45463</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>45464</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>45465</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>45466</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>45467</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>45468</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -25263,8 +24660,8 @@
   <dimension ref="A1:AD275"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A236" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B246" sqref="B246:Z252"/>
+      <pane ySplit="1" topLeftCell="A174" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A253" sqref="A253:A275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -45282,9 +44679,7 @@
       </c>
     </row>
     <row r="253" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A253" s="10">
-        <v>45454</v>
-      </c>
+      <c r="A253" s="10"/>
       <c r="B253" s="15"/>
       <c r="C253" s="15"/>
       <c r="D253" s="15"/>
@@ -45312,9 +44707,7 @@
       <c r="Z253" s="15"/>
     </row>
     <row r="254" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A254" s="10">
-        <v>45455</v>
-      </c>
+      <c r="A254" s="10"/>
       <c r="B254" s="15"/>
       <c r="C254" s="15"/>
       <c r="D254" s="15"/>
@@ -45345,9 +44738,7 @@
       <c r="AC254" s="19"/>
     </row>
     <row r="255" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A255" s="10">
-        <v>45456</v>
-      </c>
+      <c r="A255" s="10"/>
       <c r="B255" s="15"/>
       <c r="C255" s="15"/>
       <c r="D255" s="15"/>
@@ -45375,9 +44766,7 @@
       <c r="Z255" s="15"/>
     </row>
     <row r="256" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A256" s="10">
-        <v>45457</v>
-      </c>
+      <c r="A256" s="10"/>
       <c r="B256" s="15"/>
       <c r="C256" s="15"/>
       <c r="D256" s="15"/>
@@ -45405,9 +44794,7 @@
       <c r="Z256" s="15"/>
     </row>
     <row r="257" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A257" s="10">
-        <v>45458</v>
-      </c>
+      <c r="A257" s="10"/>
       <c r="B257" s="15"/>
       <c r="C257" s="15"/>
       <c r="D257" s="15"/>
@@ -45435,9 +44822,7 @@
       <c r="Z257" s="15"/>
     </row>
     <row r="258" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A258" s="10">
-        <v>45459</v>
-      </c>
+      <c r="A258" s="10"/>
       <c r="B258" s="15"/>
       <c r="C258" s="15"/>
       <c r="D258" s="15"/>
@@ -45465,9 +44850,7 @@
       <c r="Z258" s="15"/>
     </row>
     <row r="259" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A259" s="10">
-        <v>45460</v>
-      </c>
+      <c r="A259" s="10"/>
       <c r="B259" s="15"/>
       <c r="C259" s="15"/>
       <c r="D259" s="15"/>
@@ -45495,9 +44878,7 @@
       <c r="Z259" s="15"/>
     </row>
     <row r="260" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A260" s="10">
-        <v>45461</v>
-      </c>
+      <c r="A260" s="10"/>
       <c r="B260" s="15"/>
       <c r="C260" s="15"/>
       <c r="D260" s="15"/>
@@ -45525,9 +44906,7 @@
       <c r="Z260" s="15"/>
     </row>
     <row r="261" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A261" s="10">
-        <v>45462</v>
-      </c>
+      <c r="A261" s="10"/>
       <c r="B261" s="15"/>
       <c r="C261" s="15"/>
       <c r="D261" s="15"/>
@@ -45555,9 +44934,7 @@
       <c r="Z261" s="15"/>
     </row>
     <row r="262" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A262" s="10">
-        <v>45463</v>
-      </c>
+      <c r="A262" s="10"/>
       <c r="B262" s="15"/>
       <c r="C262" s="15"/>
       <c r="D262" s="15"/>
@@ -45585,9 +44962,7 @@
       <c r="Z262" s="15"/>
     </row>
     <row r="263" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A263" s="10">
-        <v>45464</v>
-      </c>
+      <c r="A263" s="10"/>
       <c r="B263" s="15"/>
       <c r="C263" s="15"/>
       <c r="D263" s="15"/>
@@ -45615,9 +44990,7 @@
       <c r="Z263" s="15"/>
     </row>
     <row r="264" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A264" s="10">
-        <v>45465</v>
-      </c>
+      <c r="A264" s="10"/>
       <c r="B264" s="15"/>
       <c r="C264" s="15"/>
       <c r="D264" s="15"/>
@@ -45645,9 +45018,7 @@
       <c r="Z264" s="15"/>
     </row>
     <row r="265" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A265" s="10">
-        <v>45466</v>
-      </c>
+      <c r="A265" s="10"/>
       <c r="B265" s="15"/>
       <c r="C265" s="15"/>
       <c r="D265" s="15"/>
@@ -45675,9 +45046,7 @@
       <c r="Z265" s="15"/>
     </row>
     <row r="266" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A266" s="10">
-        <v>45467</v>
-      </c>
+      <c r="A266" s="10"/>
       <c r="B266" s="15"/>
       <c r="C266" s="15"/>
       <c r="D266" s="15"/>
@@ -45705,9 +45074,7 @@
       <c r="Z266" s="15"/>
     </row>
     <row r="267" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A267" s="10">
-        <v>45468</v>
-      </c>
+      <c r="A267" s="10"/>
       <c r="B267" s="15"/>
       <c r="C267" s="15"/>
       <c r="D267" s="15"/>
@@ -45735,9 +45102,7 @@
       <c r="Z267" s="15"/>
     </row>
     <row r="268" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A268" s="10">
-        <v>45469</v>
-      </c>
+      <c r="A268" s="10"/>
       <c r="B268" s="15"/>
       <c r="C268" s="15"/>
       <c r="D268" s="15"/>
@@ -45765,9 +45130,7 @@
       <c r="Z268" s="15"/>
     </row>
     <row r="269" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A269" s="10">
-        <v>45470</v>
-      </c>
+      <c r="A269" s="10"/>
       <c r="B269" s="15"/>
       <c r="C269" s="15"/>
       <c r="D269" s="15"/>
@@ -45795,9 +45158,7 @@
       <c r="Z269" s="15"/>
     </row>
     <row r="270" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A270" s="10">
-        <v>45471</v>
-      </c>
+      <c r="A270" s="10"/>
       <c r="B270" s="15"/>
       <c r="C270" s="15"/>
       <c r="D270" s="15"/>
@@ -45824,9 +45185,7 @@
       <c r="Z270" s="15"/>
     </row>
     <row r="271" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A271" s="10">
-        <v>45472</v>
-      </c>
+      <c r="A271" s="10"/>
       <c r="B271" s="15"/>
       <c r="C271" s="15"/>
       <c r="D271" s="15"/>
@@ -45853,9 +45212,7 @@
       <c r="Z271" s="15"/>
     </row>
     <row r="272" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A272" s="10">
-        <v>45473</v>
-      </c>
+      <c r="A272" s="10"/>
       <c r="B272" s="15"/>
       <c r="C272" s="15"/>
       <c r="D272" s="15"/>
@@ -45882,9 +45239,7 @@
       <c r="Z272" s="15"/>
     </row>
     <row r="273" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A273" s="10">
-        <v>45474</v>
-      </c>
+      <c r="A273" s="10"/>
       <c r="B273" s="15"/>
       <c r="C273" s="15"/>
       <c r="D273" s="15"/>
@@ -45911,9 +45266,7 @@
       <c r="Z273" s="15"/>
     </row>
     <row r="274" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A274" s="10">
-        <v>45475</v>
-      </c>
+      <c r="A274" s="10"/>
       <c r="B274" s="15"/>
       <c r="C274" s="15"/>
       <c r="D274" s="15"/>
@@ -45940,9 +45293,7 @@
       <c r="Z274" s="15"/>
     </row>
     <row r="275" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A275" s="10">
-        <v>45476</v>
-      </c>
+      <c r="A275" s="10"/>
       <c r="B275" s="15"/>
       <c r="C275" s="15"/>
       <c r="D275" s="15"/>
@@ -46206,21 +45557,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001329E28168E70B428EE67616F8A60796" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="337b8eb81f7e5c21aeddc642f9582289">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a83edf6a-ab6a-4e14-b931-cd98005da12c" xmlns:ns3="20418afa-354e-465f-886d-9070cc89e96b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6e268badb0221d7eae40d2304b8be21d" ns2:_="" ns3:_="">
     <xsd:import namespace="a83edf6a-ab6a-4e14-b931-cd98005da12c"/>
@@ -46397,32 +45733,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D26EBCA7-B96E-43C0-B204-9E5DC49C44AE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="20418afa-354e-465f-886d-9070cc89e96b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a83edf6a-ab6a-4e14-b931-cd98005da12c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94E0EE0D-72B1-422E-BBC2-2D1C0AED3BC3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{135247E3-4674-49C3-8481-2C604613DBDE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -46439,4 +45765,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94E0EE0D-72B1-422E-BBC2-2D1C0AED3BC3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D26EBCA7-B96E-43C0-B204-9E5DC49C44AE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="20418afa-354e-465f-886d-9070cc89e96b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a83edf6a-ab6a-4e14-b931-cd98005da12c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>